<commit_message>
removing obsolete columns table 1
</commit_message>
<xml_diff>
--- a/1. Housebuilding (gross and rates), housing stock, demolitions, and population data, 1945-2022/England_housebuilding_stocks_population_1945_2022_CfC_release_2025_01_22.xlsx
+++ b/1. Housebuilding (gross and rates), housing stock, demolitions, and population data, 1945-2022/England_housebuilding_stocks_population_1945_2022_CfC_release_2025_01_22.xlsx
@@ -1,291 +1,295 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.breach\Documents\GitHub\local_housebuilding_1946_2022\1. Housebuilding (gross and rates), housing stock, demolitions, and population data, 1945-2022\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430CD4CD-459B-4CAD-BF3C-FDAA89084EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="England_data_table" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="population" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="stock" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="gross_total_built" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="gross_private_built" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="gross_public_built" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="England_data_table" sheetId="1" r:id="rId1"/>
+    <sheet name="population" sheetId="2" r:id="rId2"/>
+    <sheet name="stock" sheetId="3" r:id="rId3"/>
+    <sheet name="gross_total_built" sheetId="4" r:id="rId4"/>
+    <sheet name="gross_private_built" sheetId="5" r:id="rId5"/>
+    <sheet name="gross_public_built" sheetId="6" r:id="rId6"/>
   </sheets>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
-  <si>
-    <t xml:space="preserve">YEAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gross_total_built</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gross_private_built</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gross_public_built</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1945</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1946</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1947</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1948</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1949</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1950</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1951</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1952</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1953</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1954</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1955</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1956</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1957</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1958</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1959</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1960</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1961</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1962</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1963</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1964</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1966</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1967</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1968</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1969</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1970</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1971</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1972</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1973</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1974</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1975</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1976</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1977</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1978</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1979</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1982</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1983</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1988</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENGLAND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ave54_58</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="86">
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>gross_total_built</t>
+  </si>
+  <si>
+    <t>gross_private_built</t>
+  </si>
+  <si>
+    <t>gross_public_built</t>
+  </si>
+  <si>
+    <t>1945</t>
+  </si>
+  <si>
+    <t>1946</t>
+  </si>
+  <si>
+    <t>1947</t>
+  </si>
+  <si>
+    <t>1948</t>
+  </si>
+  <si>
+    <t>1949</t>
+  </si>
+  <si>
+    <t>1950</t>
+  </si>
+  <si>
+    <t>1951</t>
+  </si>
+  <si>
+    <t>1952</t>
+  </si>
+  <si>
+    <t>1953</t>
+  </si>
+  <si>
+    <t>1954</t>
+  </si>
+  <si>
+    <t>1955</t>
+  </si>
+  <si>
+    <t>1956</t>
+  </si>
+  <si>
+    <t>1957</t>
+  </si>
+  <si>
+    <t>1958</t>
+  </si>
+  <si>
+    <t>1959</t>
+  </si>
+  <si>
+    <t>1960</t>
+  </si>
+  <si>
+    <t>1961</t>
+  </si>
+  <si>
+    <t>1962</t>
+  </si>
+  <si>
+    <t>1963</t>
+  </si>
+  <si>
+    <t>1964</t>
+  </si>
+  <si>
+    <t>1965</t>
+  </si>
+  <si>
+    <t>1966</t>
+  </si>
+  <si>
+    <t>1967</t>
+  </si>
+  <si>
+    <t>1968</t>
+  </si>
+  <si>
+    <t>1969</t>
+  </si>
+  <si>
+    <t>1970</t>
+  </si>
+  <si>
+    <t>1971</t>
+  </si>
+  <si>
+    <t>1972</t>
+  </si>
+  <si>
+    <t>1973</t>
+  </si>
+  <si>
+    <t>1974</t>
+  </si>
+  <si>
+    <t>1975</t>
+  </si>
+  <si>
+    <t>1976</t>
+  </si>
+  <si>
+    <t>1977</t>
+  </si>
+  <si>
+    <t>1978</t>
+  </si>
+  <si>
+    <t>1979</t>
+  </si>
+  <si>
+    <t>1980</t>
+  </si>
+  <si>
+    <t>1981</t>
+  </si>
+  <si>
+    <t>1982</t>
+  </si>
+  <si>
+    <t>1983</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>1985</t>
+  </si>
+  <si>
+    <t>1986</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>1988</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>ENGLAND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -321,6 +325,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -602,14 +615,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -629,1553 +642,1549 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>11082355.4047285</v>
       </c>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>11123532.2403285</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>38861006</v>
       </c>
-      <c r="D3" t="n">
-        <v>41176.8356</v>
-      </c>
-      <c r="E3" t="n">
-        <v>27105.6356</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="D3">
+        <v>41176.835599999999</v>
+      </c>
+      <c r="E3">
+        <v>27105.635600000001</v>
+      </c>
+      <c r="F3">
         <v>14071.2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="n">
-        <v>11239217.2665085</v>
-      </c>
-      <c r="C4" t="n">
-        <v>39262006.4328702</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="B4">
+        <v>11239217.266508499</v>
+      </c>
+      <c r="C4">
+        <v>39262006.432870202</v>
+      </c>
+      <c r="D4">
         <v>115685.02618</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>38262.64374</v>
       </c>
-      <c r="F4" t="n">
-        <v>75482.96128</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="F4">
+        <v>75482.961280000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="n">
-        <v>11418458.1438085</v>
-      </c>
-      <c r="C5" t="n">
-        <v>39663006.8969697</v>
-      </c>
-      <c r="D5" t="n">
-        <v>179240.8773</v>
-      </c>
-      <c r="E5" t="n">
-        <v>30070.01574</v>
-      </c>
-      <c r="F5" t="n">
-        <v>149816.43584</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="B5">
+        <v>11418458.143808501</v>
+      </c>
+      <c r="C5">
+        <v>39663006.896969698</v>
+      </c>
+      <c r="D5">
+        <v>179240.87729999999</v>
+      </c>
+      <c r="E5">
+        <v>30070.015739999999</v>
+      </c>
+      <c r="F5">
+        <v>149816.43583999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="n">
-        <v>11568254.2770685</v>
-      </c>
-      <c r="C6" t="n">
-        <v>40064007.3945518</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="B6">
+        <v>11568254.277068499</v>
+      </c>
+      <c r="C6">
+        <v>40064007.394551799</v>
+      </c>
+      <c r="D6">
         <v>149796.13326</v>
       </c>
-      <c r="E6" t="n">
-        <v>23585.3245</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="E6">
+        <v>23585.324499999999</v>
+      </c>
+      <c r="F6">
         <v>126970.38728</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>11719481.9101285</v>
       </c>
-      <c r="C7" t="n">
-        <v>40465007.9280319</v>
-      </c>
-      <c r="D7" t="n">
-        <v>151227.63306</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="C7">
+        <v>40465007.928031899</v>
+      </c>
+      <c r="D7">
+        <v>151227.63305999999</v>
+      </c>
+      <c r="E7">
         <v>25078.88582</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>126683.0156</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>11864818.9287285</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>40766208.5</v>
       </c>
-      <c r="D8" t="n">
-        <v>145337.0186</v>
-      </c>
-      <c r="E8" t="n">
-        <v>19833.0186</v>
-      </c>
-      <c r="F8" t="n">
+      <c r="D8">
+        <v>145337.01860000001</v>
+      </c>
+      <c r="E8">
+        <v>19833.018599999999</v>
+      </c>
+      <c r="F8">
         <v>125504</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="n">
-        <v>12011574.845162</v>
-      </c>
-      <c r="C9" t="n">
-        <v>41020210.6181664</v>
-      </c>
-      <c r="D9" t="n">
-        <v>181567.3657</v>
-      </c>
-      <c r="E9" t="n">
-        <v>30383.2278</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="B9">
+        <v>12011574.845162001</v>
+      </c>
+      <c r="C9">
+        <v>41020210.618166402</v>
+      </c>
+      <c r="D9">
+        <v>181567.36569999999</v>
+      </c>
+      <c r="E9">
+        <v>30383.227800000001</v>
+      </c>
+      <c r="F9">
         <v>154028.16</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="n">
-        <v>12220207.1255955</v>
-      </c>
-      <c r="C10" t="n">
-        <v>41274213.2641714</v>
-      </c>
-      <c r="D10" t="n">
+      <c r="B10">
+        <v>12220207.125595501</v>
+      </c>
+      <c r="C10">
+        <v>41274213.264171399</v>
+      </c>
+      <c r="D10">
         <v>243443.7297</v>
       </c>
-      <c r="E10" t="n">
-        <v>58027.8676</v>
-      </c>
-      <c r="F10" t="n">
+      <c r="E10">
+        <v>58027.867599999998</v>
+      </c>
+      <c r="F10">
         <v>185937.84</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="n">
-        <v>12463209.6569289</v>
-      </c>
-      <c r="C11" t="n">
-        <v>41426016.5695504</v>
-      </c>
-      <c r="D11" t="n">
-        <v>277813.9806</v>
-      </c>
-      <c r="E11" t="n">
-        <v>85659.9806</v>
-      </c>
-      <c r="F11" t="n">
+      <c r="B11">
+        <v>12463209.656928901</v>
+      </c>
+      <c r="C11">
+        <v>41426016.569550402</v>
+      </c>
+      <c r="D11">
+        <v>277813.98060000001</v>
+      </c>
+      <c r="E11">
+        <v>85659.980599999995</v>
+      </c>
+      <c r="F11">
         <v>192154</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>12696801.6076624</v>
       </c>
-      <c r="C12" t="n">
-        <v>41587120.6986168</v>
-      </c>
-      <c r="D12" t="n">
-        <v>268403.4</v>
-      </c>
-      <c r="E12" t="n">
+      <c r="C12">
+        <v>41587120.698616803</v>
+      </c>
+      <c r="D12">
+        <v>268403.40000000002</v>
+      </c>
+      <c r="E12">
         <v>110773.4</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>157630</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>12930393.5583959</v>
       </c>
-      <c r="C13" t="n">
-        <v>41777925.8566301</v>
-      </c>
-      <c r="D13" t="n">
+      <c r="C13">
+        <v>41777925.856630102</v>
+      </c>
+      <c r="D13">
         <v>244860</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>115797</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>129063</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="n">
-        <v>13140415.1091294</v>
-      </c>
-      <c r="C14" t="n">
+      <c r="B14">
+        <v>13140415.109129401</v>
+      </c>
+      <c r="C14">
         <v>42052400</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>244833</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>119084</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>125749</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>13327277.6598629</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>42299600</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>221674</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>119913</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>101761</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="n">
-        <v>13524639.2105964</v>
-      </c>
-      <c r="C16" t="n">
+      <c r="B16">
+        <v>13524639.210596399</v>
+      </c>
+      <c r="C16">
         <v>42466780</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>232173</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>141508</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>90665</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>13740919.7613299</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>42759900</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>251092</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>155922</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>95170</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>13954588.3120634</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>43125300</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>248480</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>163464</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>85016</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" t="n">
-        <v>14137993.8864326</v>
-      </c>
-      <c r="C19" t="n">
+      <c r="B19">
+        <v>14137993.886432599</v>
+      </c>
+      <c r="C19">
         <v>43534400</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>254288</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>159196</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>95092</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" t="n">
-        <v>14316308.4608018</v>
-      </c>
-      <c r="C20" t="n">
+      <c r="B20">
+        <v>14316308.460801801</v>
+      </c>
+      <c r="C20">
         <v>44018300</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>249197</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>160838</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>88359</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>14554575.035171</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>44362900</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>309149</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>200643</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>108506</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>14802738.6095402</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>45081700</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>319046</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>197190</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22">
         <v>121856</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>15056895.1839095</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>45375400</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>325039</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>187885</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>137154</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>15323267.7582787</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>45681000</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>337255</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>183691</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24">
         <v>153550</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B25" t="n">
-        <v>15598644.3326479</v>
-      </c>
-      <c r="C25" t="n">
+      <c r="B25">
+        <v>15598644.332647899</v>
+      </c>
+      <c r="C25">
         <v>45871900</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25">
         <v>346259</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>203324</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25">
         <v>142935</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>15823591.2403505</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26">
         <v>45873000</v>
       </c>
-      <c r="D26" t="n">
-        <v>295829.333333333</v>
-      </c>
-      <c r="E26" t="n">
-        <v>164073.333333333</v>
-      </c>
-      <c r="F26" t="n">
+      <c r="D26">
+        <v>295829.33333333302</v>
+      </c>
+      <c r="E26">
+        <v>164073.33333333299</v>
+      </c>
+      <c r="F26">
         <v>131756</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B27" t="n">
-        <v>16039172.8147197</v>
-      </c>
-      <c r="C27" t="n">
+      <c r="B27">
+        <v>16039172.814719699</v>
+      </c>
+      <c r="C27">
         <v>46253800</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27">
         <v>286464</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27">
         <v>153321</v>
       </c>
-      <c r="F27" t="n">
+      <c r="F27">
         <v>133138</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" t="n">
-        <v>16256864.3890889</v>
-      </c>
-      <c r="C28" t="n">
+      <c r="B28">
+        <v>16256864.389088901</v>
+      </c>
+      <c r="C28">
         <v>46083600</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28">
         <v>288574</v>
       </c>
-      <c r="E28" t="n">
+      <c r="E28">
         <v>170225</v>
       </c>
-      <c r="F28" t="n">
+      <c r="F28">
         <v>118351</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
-      <c r="B29" t="n">
-        <v>16524901.3890889</v>
-      </c>
-      <c r="C29" t="n">
+      <c r="B29">
+        <v>16524901.389088901</v>
+      </c>
+      <c r="C29">
         <v>46295500</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29">
         <v>268037</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E29">
         <v>173636</v>
       </c>
-      <c r="F29" t="n">
+      <c r="F29">
         <v>94401</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
-      <c r="B30" t="n">
-        <v>16768568.3890889</v>
-      </c>
-      <c r="C30" t="n">
+      <c r="B30">
+        <v>16768568.389088901</v>
+      </c>
+      <c r="C30">
         <v>46425100</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30">
         <v>243667</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E30">
         <v>162770</v>
       </c>
-      <c r="F30" t="n">
+      <c r="F30">
         <v>81396</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" t="n">
-        <v>16790399.7567236</v>
-      </c>
-      <c r="C31" t="n">
+      <c r="B31">
+        <v>16790399.756723601</v>
+      </c>
+      <c r="C31">
         <v>46435800</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31">
         <v>222556</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E31">
         <v>120270</v>
       </c>
-      <c r="F31" t="n">
+      <c r="F31">
         <v>102286</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>16984170.569656</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32">
         <v>46453700</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32">
         <v>254901</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E32">
         <v>130791</v>
       </c>
-      <c r="F32" t="n">
+      <c r="F32">
         <v>124110</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>17180280.5426028</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33">
         <v>46417600</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33">
         <v>255649</v>
       </c>
-      <c r="E33" t="n">
+      <c r="E33">
         <v>130897</v>
       </c>
-      <c r="F33" t="n">
+      <c r="F33">
         <v>124752</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>17378788.4904854</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34">
         <v>46418700</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34">
         <v>253060</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E34">
         <v>121004</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F34">
         <v>132056</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
-      <c r="B35" t="n">
-        <v>17561681.5444642</v>
-      </c>
-      <c r="C35" t="n">
+      <c r="B35">
+        <v>17561681.544464201</v>
+      </c>
+      <c r="C35">
         <v>46351300</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35">
         <v>232997</v>
       </c>
-      <c r="E35" t="n">
+      <c r="E35">
         <v>127051</v>
       </c>
-      <c r="F35" t="n">
+      <c r="F35">
         <v>105946</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
-      <c r="B36" t="n">
-        <v>17709166.1466167</v>
-      </c>
-      <c r="C36" t="n">
+      <c r="B36">
+        <v>17709166.146616701</v>
+      </c>
+      <c r="C36">
         <v>46350700</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36">
         <v>194982</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E36">
         <v>112606</v>
       </c>
-      <c r="F36" t="n">
+      <c r="F36">
         <v>82376</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
-      <c r="B37" t="n">
-        <v>17891146.0476559</v>
-      </c>
-      <c r="C37" t="n">
+      <c r="B37">
+        <v>17891146.047655899</v>
+      </c>
+      <c r="C37">
         <v>46787200</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37">
         <v>197964</v>
       </c>
-      <c r="E37" t="n">
+      <c r="E37">
         <v>109282</v>
       </c>
-      <c r="F37" t="n">
+      <c r="F37">
         <v>88682</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
-      <c r="B38" t="n">
-        <v>18039445.88</v>
-      </c>
-      <c r="C38" t="n">
+      <c r="B38">
+        <v>18039445.879999999</v>
+      </c>
+      <c r="C38">
         <v>46819800</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38">
         <v>164646</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E38">
         <v>97844</v>
       </c>
-      <c r="F38" t="n">
+      <c r="F38">
         <v>67094.5</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
-      <c r="B39" t="n">
-        <v>18187101.9175988</v>
-      </c>
-      <c r="C39" t="n">
+      <c r="B39">
+        <v>18187101.917598799</v>
+      </c>
+      <c r="C39">
         <v>46793800</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39">
         <v>147122</v>
       </c>
-      <c r="E39" t="n">
+      <c r="E39">
         <v>106633</v>
       </c>
-      <c r="F39" t="n">
+      <c r="F39">
         <v>41246.5</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
-      <c r="B40" t="n">
-        <v>18354932.9551976</v>
-      </c>
-      <c r="C40" t="n">
+      <c r="B40">
+        <v>18354932.955197599</v>
+      </c>
+      <c r="C40">
         <v>46846700</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40">
         <v>167297</v>
       </c>
-      <c r="E40" t="n">
+      <c r="E40">
         <v>124995.5</v>
       </c>
-      <c r="F40" t="n">
+      <c r="F40">
         <v>42444</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="B41" t="n">
-        <v>18531051.4927964</v>
-      </c>
-      <c r="C41" t="n">
+      <c r="B41">
+        <v>18531051.492796399</v>
+      </c>
+      <c r="C41">
         <v>46956600</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41">
         <v>175584.5</v>
       </c>
-      <c r="E41" t="n">
+      <c r="E41">
         <v>132802.5</v>
       </c>
-      <c r="F41" t="n">
+      <c r="F41">
         <v>41653</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
-      <c r="B42" t="n">
-        <v>18701268.5303952</v>
-      </c>
-      <c r="C42" t="n">
+      <c r="B42">
+        <v>18701268.530395199</v>
+      </c>
+      <c r="C42">
         <v>47111700</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42">
         <v>169683</v>
       </c>
-      <c r="E42" t="n">
+      <c r="E42">
         <v>134720</v>
       </c>
-      <c r="F42" t="n">
+      <c r="F42">
         <v>35002.5</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
-      <c r="B43" t="n">
-        <v>18879706.067994</v>
-      </c>
-      <c r="C43" t="n">
+      <c r="B43">
+        <v>18879706.067993999</v>
+      </c>
+      <c r="C43">
         <v>47254400</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43">
         <v>177903.5</v>
       </c>
-      <c r="E43" t="n">
+      <c r="E43">
         <v>147840.5</v>
       </c>
-      <c r="F43" t="n">
+      <c r="F43">
         <v>30054</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
-      <c r="B44" t="n">
-        <v>19071076.6055928</v>
-      </c>
-      <c r="C44" t="n">
+      <c r="B44">
+        <v>19071076.605592798</v>
+      </c>
+      <c r="C44">
         <v>47406500</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44">
         <v>190836.5</v>
       </c>
-      <c r="E44" t="n">
+      <c r="E44">
         <v>160989.5</v>
       </c>
-      <c r="F44" t="n">
+      <c r="F44">
         <v>27194</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
-      <c r="B45" t="n">
-        <v>19275446.1431916</v>
-      </c>
-      <c r="C45" t="n">
+      <c r="B45">
+        <v>19275446.143191598</v>
+      </c>
+      <c r="C45">
         <v>47531300</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45">
         <v>203835.5</v>
       </c>
-      <c r="E45" t="n">
+      <c r="E45">
         <v>176280</v>
       </c>
-      <c r="F45" t="n">
+      <c r="F45">
         <v>27081.5</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
-      <c r="B46" t="n">
-        <v>19457049.6807904</v>
-      </c>
-      <c r="C46" t="n">
+      <c r="B46">
+        <v>19457049.680790398</v>
+      </c>
+      <c r="C46">
         <v>47669600</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46">
         <v>181069.5</v>
       </c>
-      <c r="E46" t="n">
+      <c r="E46">
         <v>154120</v>
       </c>
-      <c r="F46" t="n">
+      <c r="F46">
         <v>25024.5</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>51</v>
       </c>
-      <c r="B47" t="n">
-        <v>19616444.2183892</v>
-      </c>
-      <c r="C47" t="n">
+      <c r="B47">
+        <v>19616444.218389198</v>
+      </c>
+      <c r="C47">
         <v>47836200</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D47">
         <v>158860.5</v>
       </c>
-      <c r="E47" t="n">
+      <c r="E47">
         <v>130610.5</v>
       </c>
-      <c r="F47" t="n">
+      <c r="F47">
         <v>27856.5</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
-      <c r="B48" t="n">
-        <v>19764382.255988</v>
-      </c>
-      <c r="C48" t="n">
+      <c r="B48">
+        <v>19764382.255988002</v>
+      </c>
+      <c r="C48">
         <v>47828000</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48">
         <v>147404</v>
       </c>
-      <c r="E48" t="n">
+      <c r="E48">
         <v>124590.5</v>
       </c>
-      <c r="F48" t="n">
+      <c r="F48">
         <v>22961</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
-      <c r="B49" t="n">
-        <v>19912973.9328892</v>
-      </c>
-      <c r="C49" t="n">
+      <c r="B49">
+        <v>19912973.932889201</v>
+      </c>
+      <c r="C49">
         <v>47997973</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49">
         <v>155646.25</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E49">
         <v>118632</v>
       </c>
-      <c r="F49" t="n">
+      <c r="F49">
         <v>36491.75</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>54</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>20063390.1097904</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50">
         <v>48102319</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50">
         <v>157470.75</v>
       </c>
-      <c r="E50" t="n">
+      <c r="E50">
         <v>115442.5</v>
       </c>
-      <c r="F50" t="n">
+      <c r="F50">
         <v>42031.75</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>55</v>
       </c>
-      <c r="B51" t="n">
-        <v>20221833.2866916</v>
-      </c>
-      <c r="C51" t="n">
+      <c r="B51">
+        <v>20221833.286691599</v>
+      </c>
+      <c r="C51">
         <v>48228781</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D51">
         <v>165497.75</v>
       </c>
-      <c r="E51" t="n">
+      <c r="E51">
         <v>122047.5</v>
       </c>
-      <c r="F51" t="n">
+      <c r="F51">
         <v>43460.25</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>56</v>
       </c>
-      <c r="B52" t="n">
-        <v>20387140.9635928</v>
-      </c>
-      <c r="C52" t="n">
+      <c r="B52">
+        <v>20387140.963592801</v>
+      </c>
+      <c r="C52">
         <v>48383461</v>
       </c>
-      <c r="D52" t="n">
+      <c r="D52">
         <v>172362.25</v>
       </c>
-      <c r="E52" t="n">
+      <c r="E52">
         <v>123960</v>
       </c>
-      <c r="F52" t="n">
+      <c r="F52">
         <v>48432.25</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>57</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>20536662.640494</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53">
         <v>48519129</v>
       </c>
-      <c r="D53" t="n">
+      <c r="D53">
         <v>156576.25</v>
       </c>
-      <c r="E53" t="n">
+      <c r="E53">
         <v>118897.5</v>
       </c>
-      <c r="F53" t="n">
+      <c r="F53">
         <v>37697.5</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>58</v>
       </c>
-      <c r="B54" t="n">
-        <v>20683244.5673952</v>
-      </c>
-      <c r="C54" t="n">
+      <c r="B54">
+        <v>20683244.567395199</v>
+      </c>
+      <c r="C54">
         <v>48664777</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D54">
         <v>153636.5</v>
       </c>
-      <c r="E54" t="n">
+      <c r="E54">
         <v>124097.25</v>
       </c>
-      <c r="F54" t="n">
+      <c r="F54">
         <v>29559.25</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>59</v>
       </c>
-      <c r="B55" t="n">
-        <v>20815954.7442964</v>
-      </c>
-      <c r="C55" t="n">
+      <c r="B55">
+        <v>20815954.744296402</v>
+      </c>
+      <c r="C55">
         <v>48820583</v>
       </c>
-      <c r="D55" t="n">
+      <c r="D55">
         <v>139764.75</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E55">
         <v>117231.75</v>
       </c>
-      <c r="F55" t="n">
+      <c r="F55">
         <v>26960.5</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
-      <c r="B56" t="n">
-        <v>20948159.1711976</v>
-      </c>
-      <c r="C56" t="n">
+      <c r="B56">
+        <v>20948159.171197601</v>
+      </c>
+      <c r="C56">
         <v>49032872</v>
       </c>
-      <c r="D56" t="n">
+      <c r="D56">
         <v>139259</v>
       </c>
-      <c r="E56" t="n">
+      <c r="E56">
         <v>115858.5</v>
       </c>
-      <c r="F56" t="n">
+      <c r="F56">
         <v>23403</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>21076323.3480988</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57">
         <v>49233311</v>
       </c>
-      <c r="D57" t="n">
+      <c r="D57">
         <v>135218.75</v>
       </c>
-      <c r="E57" t="n">
+      <c r="E57">
         <v>113860.5</v>
       </c>
-      <c r="F57" t="n">
+      <c r="F57">
         <v>21278.25</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>62</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>21206812</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58">
         <v>49449746</v>
       </c>
-      <c r="D58" t="n">
-        <v>137482.846515753</v>
-      </c>
-      <c r="E58" t="n">
-        <v>116188.19486532</v>
-      </c>
-      <c r="F58" t="n">
+      <c r="D58">
+        <v>137482.84651575299</v>
+      </c>
+      <c r="E58">
+        <v>116188.19486531999</v>
+      </c>
+      <c r="F58">
         <v>21534</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>63</v>
       </c>
-      <c r="B59" t="n">
-        <v>21353516.4184358</v>
-      </c>
-      <c r="C59" t="n">
+      <c r="B59">
+        <v>21353516.418435801</v>
+      </c>
+      <c r="C59">
         <v>49679267</v>
       </c>
-      <c r="D59" t="n">
+      <c r="D59">
         <v>144088.210728315</v>
       </c>
-      <c r="E59" t="n">
+      <c r="E59">
         <v>123112.162117204</v>
       </c>
-      <c r="F59" t="n">
+      <c r="F59">
         <v>21256.75</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>64</v>
       </c>
-      <c r="B60" t="n">
-        <v>21513391.3368715</v>
-      </c>
-      <c r="C60" t="n">
+      <c r="B60">
+        <v>21513391.336871501</v>
+      </c>
+      <c r="C60">
         <v>49925517</v>
       </c>
-      <c r="D60" t="n">
+      <c r="D60">
         <v>151947.091700738</v>
       </c>
-      <c r="E60" t="n">
+      <c r="E60">
         <v>129517.490179574</v>
       </c>
-      <c r="F60" t="n">
+      <c r="F60">
         <v>23190</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>65</v>
       </c>
-      <c r="B61" t="n">
-        <v>21684360.2553073</v>
-      </c>
-      <c r="C61" t="n">
+      <c r="B61">
+        <v>21684360.255307298</v>
+      </c>
+      <c r="C61">
         <v>50194600</v>
       </c>
-      <c r="D61" t="n">
-        <v>162565.868837181</v>
-      </c>
-      <c r="E61" t="n">
+      <c r="D61">
+        <v>162565.86883718101</v>
+      </c>
+      <c r="E61">
         <v>136945.195556758</v>
       </c>
-      <c r="F61" t="n">
+      <c r="F61">
         <v>26168.75</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>66</v>
       </c>
-      <c r="B62" t="n">
-        <v>21869912.9894292</v>
-      </c>
-      <c r="C62" t="n">
+      <c r="B62">
+        <v>21869912.989429198</v>
+      </c>
+      <c r="C62">
         <v>50606034</v>
       </c>
-      <c r="D62" t="n">
-        <v>174561.041972302</v>
-      </c>
-      <c r="E62" t="n">
-        <v>143222.317765953</v>
-      </c>
-      <c r="F62" t="n">
+      <c r="D62">
+        <v>174561.04197230199</v>
+      </c>
+      <c r="E62">
+        <v>143222.31776595299</v>
+      </c>
+      <c r="F62">
         <v>31687.75</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>67</v>
       </c>
-      <c r="B63" t="n">
-        <v>22072565.9078649</v>
-      </c>
-      <c r="C63" t="n">
+      <c r="B63">
+        <v>22072565.907864898</v>
+      </c>
+      <c r="C63">
         <v>50965186</v>
       </c>
-      <c r="D63" t="n">
+      <c r="D63">
         <v>178022.767190757</v>
       </c>
-      <c r="E63" t="n">
+      <c r="E63">
         <v>142758.10052409</v>
       </c>
-      <c r="F63" t="n">
+      <c r="F63">
         <v>35350.75</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>68</v>
       </c>
-      <c r="B64" t="n">
-        <v>22287501.8263007</v>
-      </c>
-      <c r="C64" t="n">
+      <c r="B64">
+        <v>22287501.826300699</v>
+      </c>
+      <c r="C64">
         <v>51381093</v>
       </c>
-      <c r="D64" t="n">
+      <c r="D64">
         <v>185698.097237254</v>
       </c>
-      <c r="E64" t="n">
-        <v>143397.902792809</v>
-      </c>
-      <c r="F64" t="n">
+      <c r="E64">
+        <v>143397.90279280901</v>
+      </c>
+      <c r="F64">
         <v>42145</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>69</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65">
         <v>22511035.7447365</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65">
         <v>51815853</v>
       </c>
-      <c r="D65" t="n">
-        <v>164710.288064173</v>
-      </c>
-      <c r="E65" t="n">
-        <v>120474.186873697</v>
-      </c>
-      <c r="F65" t="n">
+      <c r="D65">
+        <v>164710.28806417299</v>
+      </c>
+      <c r="E65">
+        <v>120474.18687369701</v>
+      </c>
+      <c r="F65">
         <v>44260.75</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>70</v>
       </c>
-      <c r="B66" t="n">
-        <v>22693802.4821061</v>
-      </c>
-      <c r="C66" t="n">
+      <c r="B66">
+        <v>22693802.482106101</v>
+      </c>
+      <c r="C66">
         <v>52196381</v>
       </c>
-      <c r="D66" t="n">
-        <v>143869.42074515</v>
-      </c>
-      <c r="E66" t="n">
-        <v>97117.9028880071</v>
-      </c>
-      <c r="F66" t="n">
+      <c r="D66">
+        <v>143869.42074515001</v>
+      </c>
+      <c r="E66">
+        <v>97117.902888007098</v>
+      </c>
+      <c r="F66">
         <v>47122.25</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>71</v>
       </c>
-      <c r="B67" t="n">
-        <v>22838672.4005418</v>
-      </c>
-      <c r="C67" t="n">
+      <c r="B67">
+        <v>22838672.400541801</v>
+      </c>
+      <c r="C67">
         <v>52642452</v>
       </c>
-      <c r="D67" t="n">
-        <v>124335.117267249</v>
-      </c>
-      <c r="E67" t="n">
-        <v>86068.1767910587</v>
-      </c>
-      <c r="F67" t="n">
+      <c r="D67">
+        <v>124335.11726724901</v>
+      </c>
+      <c r="E67">
+        <v>86068.176791058693</v>
+      </c>
+      <c r="F67">
         <v>51903.25</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>72</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68">
         <v>22976066</v>
       </c>
-      <c r="C68" t="n">
+      <c r="C68">
         <v>53107169</v>
       </c>
-      <c r="D68" t="n">
-        <v>135355.745647614</v>
-      </c>
-      <c r="E68" t="n">
-        <v>86818.8408857089</v>
-      </c>
-      <c r="F68" t="n">
+      <c r="D68">
+        <v>135355.74564761401</v>
+      </c>
+      <c r="E68">
+        <v>86818.840885708894</v>
+      </c>
+      <c r="F68">
         <v>53066.5</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>73</v>
       </c>
-      <c r="B69" t="n">
-        <v>23116851.0133085</v>
-      </c>
-      <c r="C69" t="n">
+      <c r="B69">
+        <v>23116851.013308499</v>
+      </c>
+      <c r="C69">
         <v>53506812</v>
       </c>
-      <c r="D69" t="n">
+      <c r="D69">
         <v>127606.5</v>
       </c>
-      <c r="E69" t="n">
+      <c r="E69">
         <v>84832.5</v>
       </c>
-      <c r="F69" t="n">
+      <c r="F69">
         <v>42886.5</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>74</v>
       </c>
-      <c r="B70" t="n">
-        <v>23247462.1229409</v>
-      </c>
-      <c r="C70" t="n">
+      <c r="B70">
+        <v>23247462.122940902</v>
+      </c>
+      <c r="C70">
         <v>53918686</v>
       </c>
-      <c r="D70" t="n">
+      <c r="D70">
         <v>125399</v>
       </c>
-      <c r="E70" t="n">
+      <c r="E70">
         <v>88062.5</v>
       </c>
-      <c r="F70" t="n">
+      <c r="F70">
         <v>37454</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>75</v>
       </c>
-      <c r="B71" t="n">
-        <v>23389956.2325733</v>
-      </c>
-      <c r="C71" t="n">
+      <c r="B71">
+        <v>23389956.232573301</v>
+      </c>
+      <c r="C71">
         <v>54370319</v>
       </c>
-      <c r="D71" t="n">
+      <c r="D71">
         <v>147170.25</v>
       </c>
-      <c r="E71" t="n">
+      <c r="E71">
         <v>94567.5</v>
       </c>
-      <c r="F71" t="n">
+      <c r="F71">
         <v>52675.25</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>76</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72">
         <v>23566538.3422057</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72">
         <v>54808676</v>
       </c>
-      <c r="D72" t="n">
+      <c r="D72">
         <v>143899.25</v>
       </c>
-      <c r="E72" t="n">
+      <c r="E72">
         <v>107677.5</v>
       </c>
-      <c r="F72" t="n">
+      <c r="F72">
         <v>36326.75</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>77</v>
       </c>
-      <c r="B73" t="n">
-        <v>23762072.4518381</v>
-      </c>
-      <c r="C73" t="n">
+      <c r="B73">
+        <v>23762072.451838098</v>
+      </c>
+      <c r="C73">
         <v>55289034</v>
       </c>
-      <c r="D73" t="n">
+      <c r="D73">
         <v>153373</v>
       </c>
-      <c r="E73" t="n">
+      <c r="E73">
         <v>117517.5</v>
       </c>
-      <c r="F73" t="n">
+      <c r="F73">
         <v>36035.5</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>78</v>
       </c>
-      <c r="B74" t="n">
-        <v>23985306.5614705</v>
-      </c>
-      <c r="C74" t="n">
+      <c r="B74">
+        <v>23985306.561470501</v>
+      </c>
+      <c r="C74">
         <v>55619548</v>
       </c>
-      <c r="D74" t="n">
+      <c r="D74">
         <v>169798.5</v>
       </c>
-      <c r="E74" t="n">
+      <c r="E74">
         <v>128237.5</v>
       </c>
-      <c r="F74" t="n">
+      <c r="F74">
         <v>41753.5</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>79</v>
       </c>
-      <c r="B75" t="n">
-        <v>24213476.6711028</v>
-      </c>
-      <c r="C75" t="n">
+      <c r="B75">
+        <v>24213476.671102799</v>
+      </c>
+      <c r="C75">
         <v>55924528</v>
       </c>
-      <c r="D75" t="n">
+      <c r="D75">
         <v>185250.5</v>
       </c>
-      <c r="E75" t="n">
+      <c r="E75">
         <v>135077.5</v>
       </c>
-      <c r="F75" t="n">
+      <c r="F75">
         <v>50235.5</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>80</v>
       </c>
-      <c r="B76" t="n">
-        <v>24461242.7807352</v>
-      </c>
-      <c r="C76" t="n">
+      <c r="B76">
+        <v>24461242.780735198</v>
+      </c>
+      <c r="C76">
         <v>56230056</v>
       </c>
-      <c r="D76" t="n">
+      <c r="D76">
         <v>191992.5</v>
       </c>
-      <c r="E76" t="n">
+      <c r="E76">
         <v>138842.5</v>
       </c>
-      <c r="F76" t="n">
+      <c r="F76">
         <v>53252.5</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>81</v>
       </c>
-      <c r="B77" t="n">
-        <v>24709833.8903676</v>
-      </c>
-      <c r="C77" t="n">
+      <c r="B77">
+        <v>24709833.890367601</v>
+      </c>
+      <c r="C77">
         <v>56325961</v>
       </c>
-      <c r="D77" t="n">
+      <c r="D77">
         <v>175920</v>
       </c>
-      <c r="E77" t="n">
+      <c r="E77">
         <v>128732.5</v>
       </c>
-      <c r="F77" t="n">
+      <c r="F77">
         <v>47400</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>82</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78">
         <v>24927588</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78">
         <v>56554891</v>
       </c>
-      <c r="D78" t="n">
+      <c r="D78">
         <v>185533</v>
       </c>
-      <c r="E78" t="n">
+      <c r="E78">
         <v>134142.5</v>
       </c>
-      <c r="F78" t="n">
+      <c r="F78">
         <v>51653</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:BZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -2411,257 +2420,257 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>38861006</v>
       </c>
-      <c r="C2" t="n">
-        <v>39262006.4328702</v>
-      </c>
-      <c r="D2" t="n">
-        <v>39663006.8969697</v>
-      </c>
-      <c r="E2" t="n">
-        <v>40064007.3945518</v>
-      </c>
-      <c r="F2" t="n">
-        <v>40465007.9280319</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="C2">
+        <v>39262006.432870202</v>
+      </c>
+      <c r="D2">
+        <v>39663006.896969698</v>
+      </c>
+      <c r="E2">
+        <v>40064007.394551799</v>
+      </c>
+      <c r="F2">
+        <v>40465007.928031899</v>
+      </c>
+      <c r="G2">
         <v>40766208.5</v>
       </c>
-      <c r="H2" t="n">
-        <v>41020210.6181664</v>
-      </c>
-      <c r="I2" t="n">
-        <v>41274213.2641714</v>
-      </c>
-      <c r="J2" t="n">
-        <v>41426016.5695504</v>
-      </c>
-      <c r="K2" t="n">
-        <v>41587120.6986168</v>
-      </c>
-      <c r="L2" t="n">
-        <v>41777925.8566301</v>
-      </c>
-      <c r="M2" t="n">
+      <c r="H2">
+        <v>41020210.618166402</v>
+      </c>
+      <c r="I2">
+        <v>41274213.264171399</v>
+      </c>
+      <c r="J2">
+        <v>41426016.569550402</v>
+      </c>
+      <c r="K2">
+        <v>41587120.698616803</v>
+      </c>
+      <c r="L2">
+        <v>41777925.856630102</v>
+      </c>
+      <c r="M2">
         <v>42052400</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>42299600</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>42466780</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2">
         <v>42759900</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2">
         <v>43125300</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2">
         <v>43534400</v>
       </c>
-      <c r="S2" t="n">
+      <c r="S2">
         <v>44018300</v>
       </c>
-      <c r="T2" t="n">
+      <c r="T2">
         <v>44362900</v>
       </c>
-      <c r="U2" t="n">
+      <c r="U2">
         <v>45081700</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V2">
         <v>45375400</v>
       </c>
-      <c r="W2" t="n">
+      <c r="W2">
         <v>45681000</v>
       </c>
-      <c r="X2" t="n">
+      <c r="X2">
         <v>45871900</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="Y2">
         <v>45873000</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="Z2">
         <v>46253800</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AA2">
         <v>46083600</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AB2">
         <v>46295500</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AC2">
         <v>46425100</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AD2">
         <v>46435800</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AE2">
         <v>46453700</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2">
         <v>46417600</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG2">
         <v>46418700</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AH2">
         <v>46351300</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AI2">
         <v>46350700</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AJ2">
         <v>46787200</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AK2">
         <v>46819800</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="AL2">
         <v>46793800</v>
       </c>
-      <c r="AM2" t="n">
+      <c r="AM2">
         <v>46846700</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="AN2">
         <v>46956600</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="AO2">
         <v>47111700</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="AP2">
         <v>47254400</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AQ2">
         <v>47406500</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AR2">
         <v>47531300</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="AS2">
         <v>47669600</v>
       </c>
-      <c r="AT2" t="n">
+      <c r="AT2">
         <v>47836200</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="AU2">
         <v>47828000</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="AV2">
         <v>47997973</v>
       </c>
-      <c r="AW2" t="n">
+      <c r="AW2">
         <v>48102319</v>
       </c>
-      <c r="AX2" t="n">
+      <c r="AX2">
         <v>48228781</v>
       </c>
-      <c r="AY2" t="n">
+      <c r="AY2">
         <v>48383461</v>
       </c>
-      <c r="AZ2" t="n">
+      <c r="AZ2">
         <v>48519129</v>
       </c>
-      <c r="BA2" t="n">
+      <c r="BA2">
         <v>48664777</v>
       </c>
-      <c r="BB2" t="n">
+      <c r="BB2">
         <v>48820583</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="BC2">
         <v>49032872</v>
       </c>
-      <c r="BD2" t="n">
+      <c r="BD2">
         <v>49233311</v>
       </c>
-      <c r="BE2" t="n">
+      <c r="BE2">
         <v>49449746</v>
       </c>
-      <c r="BF2" t="n">
+      <c r="BF2">
         <v>49679267</v>
       </c>
-      <c r="BG2" t="n">
+      <c r="BG2">
         <v>49925517</v>
       </c>
-      <c r="BH2" t="n">
+      <c r="BH2">
         <v>50194600</v>
       </c>
-      <c r="BI2" t="n">
+      <c r="BI2">
         <v>50606034</v>
       </c>
-      <c r="BJ2" t="n">
+      <c r="BJ2">
         <v>50965186</v>
       </c>
-      <c r="BK2" t="n">
+      <c r="BK2">
         <v>51381093</v>
       </c>
-      <c r="BL2" t="n">
+      <c r="BL2">
         <v>51815853</v>
       </c>
-      <c r="BM2" t="n">
+      <c r="BM2">
         <v>52196381</v>
       </c>
-      <c r="BN2" t="n">
+      <c r="BN2">
         <v>52642452</v>
       </c>
-      <c r="BO2" t="n">
+      <c r="BO2">
         <v>53107169</v>
       </c>
-      <c r="BP2" t="n">
+      <c r="BP2">
         <v>53506812</v>
       </c>
-      <c r="BQ2" t="n">
+      <c r="BQ2">
         <v>53918686</v>
       </c>
-      <c r="BR2" t="n">
+      <c r="BR2">
         <v>54370319</v>
       </c>
-      <c r="BS2" t="n">
+      <c r="BS2">
         <v>54808676</v>
       </c>
-      <c r="BT2" t="n">
+      <c r="BT2">
         <v>55289034</v>
       </c>
-      <c r="BU2" t="n">
+      <c r="BU2">
         <v>55619548</v>
       </c>
-      <c r="BV2" t="n">
+      <c r="BV2">
         <v>55924528</v>
       </c>
-      <c r="BW2" t="n">
+      <c r="BW2">
         <v>56230056</v>
       </c>
-      <c r="BX2" t="n">
+      <c r="BX2">
         <v>56325961</v>
       </c>
-      <c r="BY2" t="n">
+      <c r="BY2">
         <v>56554891</v>
       </c>
-      <c r="BZ2" t="n">
+      <c r="BZ2">
         <v>57106398</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:BZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -2897,257 +2906,259 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>11082355.4047285</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>11123532.2403285</v>
       </c>
-      <c r="D2" t="n">
-        <v>11239217.2665085</v>
-      </c>
-      <c r="E2" t="n">
-        <v>11418458.1438085</v>
-      </c>
-      <c r="F2" t="n">
-        <v>11568254.2770685</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="D2">
+        <v>11239217.266508499</v>
+      </c>
+      <c r="E2">
+        <v>11418458.143808501</v>
+      </c>
+      <c r="F2">
+        <v>11568254.277068499</v>
+      </c>
+      <c r="G2">
         <v>11719481.9101285</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>11864818.9287285</v>
       </c>
-      <c r="I2" t="n">
-        <v>12011574.845162</v>
-      </c>
-      <c r="J2" t="n">
-        <v>12220207.1255955</v>
-      </c>
-      <c r="K2" t="n">
-        <v>12463209.6569289</v>
-      </c>
-      <c r="L2" t="n">
+      <c r="I2">
+        <v>12011574.845162001</v>
+      </c>
+      <c r="J2">
+        <v>12220207.125595501</v>
+      </c>
+      <c r="K2">
+        <v>12463209.656928901</v>
+      </c>
+      <c r="L2">
         <v>12696801.6076624</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>12930393.5583959</v>
       </c>
-      <c r="N2" t="n">
-        <v>13140415.1091294</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="N2">
+        <v>13140415.109129401</v>
+      </c>
+      <c r="O2">
         <v>13327277.6598629</v>
       </c>
-      <c r="P2" t="n">
-        <v>13524639.2105964</v>
-      </c>
-      <c r="Q2" t="n">
+      <c r="P2">
+        <v>13524639.210596399</v>
+      </c>
+      <c r="Q2">
         <v>13740919.7613299</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2">
         <v>13954588.3120634</v>
       </c>
-      <c r="S2" t="n">
-        <v>14137993.8864326</v>
-      </c>
-      <c r="T2" t="n">
-        <v>14316308.4608018</v>
-      </c>
-      <c r="U2" t="n">
+      <c r="S2">
+        <v>14137993.886432599</v>
+      </c>
+      <c r="T2">
+        <v>14316308.460801801</v>
+      </c>
+      <c r="U2">
         <v>14554575.035171</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V2">
         <v>14802738.6095402</v>
       </c>
-      <c r="W2" t="n">
+      <c r="W2">
         <v>15056895.1839095</v>
       </c>
-      <c r="X2" t="n">
+      <c r="X2">
         <v>15323267.7582787</v>
       </c>
-      <c r="Y2" t="n">
-        <v>15598644.3326479</v>
-      </c>
-      <c r="Z2" t="n">
+      <c r="Y2">
+        <v>15598644.332647899</v>
+      </c>
+      <c r="Z2">
         <v>15823591.2403505</v>
       </c>
-      <c r="AA2" t="n">
-        <v>16039172.8147197</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>16256864.3890889</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>16524901.3890889</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>16768568.3890889</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>16790399.7567236</v>
-      </c>
-      <c r="AF2" t="n">
+      <c r="AA2">
+        <v>16039172.814719699</v>
+      </c>
+      <c r="AB2">
+        <v>16256864.389088901</v>
+      </c>
+      <c r="AC2">
+        <v>16524901.389088901</v>
+      </c>
+      <c r="AD2">
+        <v>16768568.389088901</v>
+      </c>
+      <c r="AE2">
+        <v>16790399.756723601</v>
+      </c>
+      <c r="AF2">
         <v>16984170.569656</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG2">
         <v>17180280.5426028</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AH2">
         <v>17378788.4904854</v>
       </c>
-      <c r="AI2" t="n">
-        <v>17561681.5444642</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>17709166.1466167</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>17891146.0476559</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>18039445.88</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>18187101.9175988</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>18354932.9551976</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>18531051.4927964</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>18701268.5303952</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>18879706.067994</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>19071076.6055928</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>19275446.1431916</v>
-      </c>
-      <c r="AT2" t="n">
-        <v>19457049.6807904</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>19616444.2183892</v>
-      </c>
-      <c r="AV2" t="n">
-        <v>19764382.255988</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>19912973.9328892</v>
-      </c>
-      <c r="AX2" t="n">
+      <c r="AI2">
+        <v>17561681.544464201</v>
+      </c>
+      <c r="AJ2">
+        <v>17709166.146616701</v>
+      </c>
+      <c r="AK2">
+        <v>17891146.047655899</v>
+      </c>
+      <c r="AL2">
+        <v>18039445.879999999</v>
+      </c>
+      <c r="AM2">
+        <v>18187101.917598799</v>
+      </c>
+      <c r="AN2">
+        <v>18354932.955197599</v>
+      </c>
+      <c r="AO2">
+        <v>18531051.492796399</v>
+      </c>
+      <c r="AP2">
+        <v>18701268.530395199</v>
+      </c>
+      <c r="AQ2">
+        <v>18879706.067993999</v>
+      </c>
+      <c r="AR2">
+        <v>19071076.605592798</v>
+      </c>
+      <c r="AS2">
+        <v>19275446.143191598</v>
+      </c>
+      <c r="AT2">
+        <v>19457049.680790398</v>
+      </c>
+      <c r="AU2">
+        <v>19616444.218389198</v>
+      </c>
+      <c r="AV2">
+        <v>19764382.255988002</v>
+      </c>
+      <c r="AW2">
+        <v>19912973.932889201</v>
+      </c>
+      <c r="AX2">
         <v>20063390.1097904</v>
       </c>
-      <c r="AY2" t="n">
-        <v>20221833.2866916</v>
-      </c>
-      <c r="AZ2" t="n">
-        <v>20387140.9635928</v>
-      </c>
-      <c r="BA2" t="n">
+      <c r="AY2">
+        <v>20221833.286691599</v>
+      </c>
+      <c r="AZ2">
+        <v>20387140.963592801</v>
+      </c>
+      <c r="BA2">
         <v>20536662.640494</v>
       </c>
-      <c r="BB2" t="n">
-        <v>20683244.5673952</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>20815954.7442964</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>20948159.1711976</v>
-      </c>
-      <c r="BE2" t="n">
+      <c r="BB2">
+        <v>20683244.567395199</v>
+      </c>
+      <c r="BC2">
+        <v>20815954.744296402</v>
+      </c>
+      <c r="BD2">
+        <v>20948159.171197601</v>
+      </c>
+      <c r="BE2">
         <v>21076323.3480988</v>
       </c>
-      <c r="BF2" t="n">
+      <c r="BF2">
         <v>21206812</v>
       </c>
-      <c r="BG2" t="n">
-        <v>21353516.4184358</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>21513391.3368715</v>
-      </c>
-      <c r="BI2" t="n">
-        <v>21684360.2553073</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>21869912.9894292</v>
-      </c>
-      <c r="BK2" t="n">
-        <v>22072565.9078649</v>
-      </c>
-      <c r="BL2" t="n">
-        <v>22287501.8263007</v>
-      </c>
-      <c r="BM2" t="n">
+      <c r="BG2">
+        <v>21353516.418435801</v>
+      </c>
+      <c r="BH2">
+        <v>21513391.336871501</v>
+      </c>
+      <c r="BI2">
+        <v>21684360.255307298</v>
+      </c>
+      <c r="BJ2">
+        <v>21869912.989429198</v>
+      </c>
+      <c r="BK2">
+        <v>22072565.907864898</v>
+      </c>
+      <c r="BL2">
+        <v>22287501.826300699</v>
+      </c>
+      <c r="BM2">
         <v>22511035.7447365</v>
       </c>
-      <c r="BN2" t="n">
-        <v>22693802.4821061</v>
-      </c>
-      <c r="BO2" t="n">
-        <v>22838672.4005418</v>
-      </c>
-      <c r="BP2" t="n">
+      <c r="BN2">
+        <v>22693802.482106101</v>
+      </c>
+      <c r="BO2">
+        <v>22838672.400541801</v>
+      </c>
+      <c r="BP2">
         <v>22976066</v>
       </c>
-      <c r="BQ2" t="n">
-        <v>23116851.0133085</v>
-      </c>
-      <c r="BR2" t="n">
-        <v>23247462.1229409</v>
-      </c>
-      <c r="BS2" t="n">
-        <v>23389956.2325733</v>
-      </c>
-      <c r="BT2" t="n">
+      <c r="BQ2">
+        <v>23116851.013308499</v>
+      </c>
+      <c r="BR2">
+        <v>23247462.122940902</v>
+      </c>
+      <c r="BS2">
+        <v>23389956.232573301</v>
+      </c>
+      <c r="BT2">
         <v>23566538.3422057</v>
       </c>
-      <c r="BU2" t="n">
-        <v>23762072.4518381</v>
-      </c>
-      <c r="BV2" t="n">
-        <v>23985306.5614705</v>
-      </c>
-      <c r="BW2" t="n">
-        <v>24213476.6711028</v>
-      </c>
-      <c r="BX2" t="n">
-        <v>24461242.7807352</v>
-      </c>
-      <c r="BY2" t="n">
-        <v>24709833.8903676</v>
-      </c>
-      <c r="BZ2" t="n">
+      <c r="BU2">
+        <v>23762072.451838098</v>
+      </c>
+      <c r="BV2">
+        <v>23985306.561470501</v>
+      </c>
+      <c r="BW2">
+        <v>24213476.671102799</v>
+      </c>
+      <c r="BX2">
+        <v>24461242.780735198</v>
+      </c>
+      <c r="BY2">
+        <v>24709833.890367601</v>
+      </c>
+      <c r="BZ2">
         <v>24927588</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:BZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3383,257 +3394,259 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="n">
-        <v>41176.8356</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>41176.835599999999</v>
+      </c>
+      <c r="C2">
         <v>115685.02618</v>
       </c>
-      <c r="D2" t="n">
-        <v>179240.8773</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="D2">
+        <v>179240.87729999999</v>
+      </c>
+      <c r="E2">
         <v>149796.13326</v>
       </c>
-      <c r="F2" t="n">
-        <v>151227.63306</v>
-      </c>
-      <c r="G2" t="n">
-        <v>145337.0186</v>
-      </c>
-      <c r="H2" t="n">
-        <v>181567.3657</v>
-      </c>
-      <c r="I2" t="n">
+      <c r="F2">
+        <v>151227.63305999999</v>
+      </c>
+      <c r="G2">
+        <v>145337.01860000001</v>
+      </c>
+      <c r="H2">
+        <v>181567.36569999999</v>
+      </c>
+      <c r="I2">
         <v>243443.7297</v>
       </c>
-      <c r="J2" t="n">
-        <v>277813.9806</v>
-      </c>
-      <c r="K2" t="n">
-        <v>268403.4</v>
-      </c>
-      <c r="L2" t="n">
+      <c r="J2">
+        <v>277813.98060000001</v>
+      </c>
+      <c r="K2">
+        <v>268403.40000000002</v>
+      </c>
+      <c r="L2">
         <v>244860</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>244833</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>221674</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>232173</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2">
         <v>251092</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2">
         <v>248480</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2">
         <v>254288</v>
       </c>
-      <c r="S2" t="n">
+      <c r="S2">
         <v>249197</v>
       </c>
-      <c r="T2" t="n">
+      <c r="T2">
         <v>309149</v>
       </c>
-      <c r="U2" t="n">
+      <c r="U2">
         <v>319046</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V2">
         <v>325039</v>
       </c>
-      <c r="W2" t="n">
+      <c r="W2">
         <v>337255</v>
       </c>
-      <c r="X2" t="n">
+      <c r="X2">
         <v>346259</v>
       </c>
-      <c r="Y2" t="n">
-        <v>295829.333333333</v>
-      </c>
-      <c r="Z2" t="n">
+      <c r="Y2">
+        <v>295829.33333333302</v>
+      </c>
+      <c r="Z2">
         <v>286464</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AA2">
         <v>288574</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AB2">
         <v>268037</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AC2">
         <v>243667</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AD2">
         <v>222556</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AE2">
         <v>254901</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2">
         <v>255649</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG2">
         <v>253060</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AH2">
         <v>232997</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AI2">
         <v>194982</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AJ2">
         <v>197964</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AK2">
         <v>164646</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="AL2">
         <v>147122</v>
       </c>
-      <c r="AM2" t="n">
+      <c r="AM2">
         <v>167297</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="AN2">
         <v>175584.5</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="AO2">
         <v>169683</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="AP2">
         <v>177903.5</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AQ2">
         <v>190836.5</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AR2">
         <v>203835.5</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="AS2">
         <v>181069.5</v>
       </c>
-      <c r="AT2" t="n">
+      <c r="AT2">
         <v>158860.5</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="AU2">
         <v>147404</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="AV2">
         <v>155646.25</v>
       </c>
-      <c r="AW2" t="n">
+      <c r="AW2">
         <v>157470.75</v>
       </c>
-      <c r="AX2" t="n">
+      <c r="AX2">
         <v>165497.75</v>
       </c>
-      <c r="AY2" t="n">
+      <c r="AY2">
         <v>172362.25</v>
       </c>
-      <c r="AZ2" t="n">
+      <c r="AZ2">
         <v>156576.25</v>
       </c>
-      <c r="BA2" t="n">
+      <c r="BA2">
         <v>153636.5</v>
       </c>
-      <c r="BB2" t="n">
+      <c r="BB2">
         <v>139764.75</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="BC2">
         <v>139259</v>
       </c>
-      <c r="BD2" t="n">
+      <c r="BD2">
         <v>135218.75</v>
       </c>
-      <c r="BE2" t="n">
-        <v>137482.846515753</v>
-      </c>
-      <c r="BF2" t="n">
+      <c r="BE2">
+        <v>137482.84651575299</v>
+      </c>
+      <c r="BF2">
         <v>144088.210728315</v>
       </c>
-      <c r="BG2" t="n">
+      <c r="BG2">
         <v>151947.091700738</v>
       </c>
-      <c r="BH2" t="n">
-        <v>162565.868837181</v>
-      </c>
-      <c r="BI2" t="n">
-        <v>174561.041972302</v>
-      </c>
-      <c r="BJ2" t="n">
+      <c r="BH2">
+        <v>162565.86883718101</v>
+      </c>
+      <c r="BI2">
+        <v>174561.04197230199</v>
+      </c>
+      <c r="BJ2">
         <v>178022.767190757</v>
       </c>
-      <c r="BK2" t="n">
+      <c r="BK2">
         <v>185698.097237254</v>
       </c>
-      <c r="BL2" t="n">
-        <v>164710.288064173</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>143869.42074515</v>
-      </c>
-      <c r="BN2" t="n">
-        <v>124335.117267249</v>
-      </c>
-      <c r="BO2" t="n">
-        <v>135355.745647614</v>
-      </c>
-      <c r="BP2" t="n">
+      <c r="BL2">
+        <v>164710.28806417299</v>
+      </c>
+      <c r="BM2">
+        <v>143869.42074515001</v>
+      </c>
+      <c r="BN2">
+        <v>124335.11726724901</v>
+      </c>
+      <c r="BO2">
+        <v>135355.74564761401</v>
+      </c>
+      <c r="BP2">
         <v>127606.5</v>
       </c>
-      <c r="BQ2" t="n">
+      <c r="BQ2">
         <v>125399</v>
       </c>
-      <c r="BR2" t="n">
+      <c r="BR2">
         <v>147170.25</v>
       </c>
-      <c r="BS2" t="n">
+      <c r="BS2">
         <v>143899.25</v>
       </c>
-      <c r="BT2" t="n">
+      <c r="BT2">
         <v>153373</v>
       </c>
-      <c r="BU2" t="n">
+      <c r="BU2">
         <v>169798.5</v>
       </c>
-      <c r="BV2" t="n">
+      <c r="BV2">
         <v>185250.5</v>
       </c>
-      <c r="BW2" t="n">
+      <c r="BW2">
         <v>191992.5</v>
       </c>
-      <c r="BX2" t="n">
+      <c r="BX2">
         <v>175920</v>
       </c>
-      <c r="BY2" t="n">
+      <c r="BY2">
         <v>185533</v>
       </c>
-      <c r="BZ2" t="n">
+      <c r="BZ2">
         <v>195180</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:BZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1:AD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3722,410 +3735,406 @@
         <v>34</v>
       </c>
       <c r="AD1" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="AE1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AF1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AG1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AH1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AJ1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AK1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AL1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AM1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AN1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AO1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AP1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AQ1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AR1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AS1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AT1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AU1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AV1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AW1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AX1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AY1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AZ1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="BA1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="BB1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BC1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BD1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BE1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="BF1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="BG1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="BH1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="BI1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="BJ1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BK1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="BL1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BM1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BN1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BO1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BP1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BQ1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BR1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BS1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BT1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="BU1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="BV1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="BW1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="BX1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="BY1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="BZ1" t="s">
-        <v>82</v>
-      </c>
-      <c r="CA1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="n">
-        <v>27105.6356</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2">
+        <v>27105.635600000001</v>
+      </c>
+      <c r="C2">
         <v>38262.64374</v>
       </c>
-      <c r="D2" t="n">
-        <v>30070.01574</v>
-      </c>
-      <c r="E2" t="n">
-        <v>23585.3245</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="D2">
+        <v>30070.015739999999</v>
+      </c>
+      <c r="E2">
+        <v>23585.324499999999</v>
+      </c>
+      <c r="F2">
         <v>25078.88582</v>
       </c>
-      <c r="G2" t="n">
-        <v>19833.0186</v>
-      </c>
-      <c r="H2" t="n">
-        <v>30383.2278</v>
-      </c>
-      <c r="I2" t="n">
-        <v>58027.8676</v>
-      </c>
-      <c r="J2" t="n">
-        <v>85659.9806</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="G2">
+        <v>19833.018599999999</v>
+      </c>
+      <c r="H2">
+        <v>30383.227800000001</v>
+      </c>
+      <c r="I2">
+        <v>58027.867599999998</v>
+      </c>
+      <c r="J2">
+        <v>85659.980599999995</v>
+      </c>
+      <c r="K2">
         <v>110773.4</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>115797</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>119084</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>119913</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>141508</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2">
         <v>155922</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2">
         <v>163464</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2">
         <v>159196</v>
       </c>
-      <c r="S2" t="n">
+      <c r="S2">
         <v>160838</v>
       </c>
-      <c r="T2" t="n">
+      <c r="T2">
         <v>200643</v>
       </c>
-      <c r="U2" t="n">
+      <c r="U2">
         <v>197190</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V2">
         <v>187885</v>
       </c>
-      <c r="W2" t="n">
+      <c r="W2">
         <v>183691</v>
       </c>
-      <c r="X2" t="n">
+      <c r="X2">
         <v>203324</v>
       </c>
-      <c r="Y2" t="n">
-        <v>164073.333333333</v>
-      </c>
-      <c r="Z2" t="n">
+      <c r="Y2">
+        <v>164073.33333333299</v>
+      </c>
+      <c r="Z2">
         <v>153321</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AA2">
         <v>170225</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AB2">
         <v>173636</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AC2">
         <v>162770</v>
       </c>
-      <c r="AD2" t="n">
-        <v>110026.5</v>
-      </c>
-      <c r="AE2" t="n">
+      <c r="AD2">
         <v>120270</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AE2">
         <v>130791</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AF2">
         <v>130897</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AG2">
         <v>121004</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AH2">
         <v>127051</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AI2">
         <v>112606</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AJ2">
         <v>109282</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="AK2">
         <v>97844</v>
       </c>
-      <c r="AM2" t="n">
+      <c r="AL2">
         <v>106633</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="AM2">
         <v>124995.5</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="AN2">
         <v>132802.5</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="AO2">
         <v>134720</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AP2">
         <v>147840.5</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AQ2">
         <v>160989.5</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="AR2">
         <v>176280</v>
       </c>
-      <c r="AT2" t="n">
+      <c r="AS2">
         <v>154120</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="AT2">
         <v>130610.5</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="AU2">
         <v>124590.5</v>
       </c>
-      <c r="AW2" t="n">
+      <c r="AV2">
         <v>118632</v>
       </c>
-      <c r="AX2" t="n">
+      <c r="AW2">
         <v>115442.5</v>
       </c>
-      <c r="AY2" t="n">
+      <c r="AX2">
         <v>122047.5</v>
       </c>
-      <c r="AZ2" t="n">
+      <c r="AY2">
         <v>123960</v>
       </c>
-      <c r="BA2" t="n">
+      <c r="AZ2">
         <v>118897.5</v>
       </c>
-      <c r="BB2" t="n">
+      <c r="BA2">
         <v>124097.25</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="BB2">
         <v>117231.75</v>
       </c>
-      <c r="BD2" t="n">
+      <c r="BC2">
         <v>115858.5</v>
       </c>
-      <c r="BE2" t="n">
+      <c r="BD2">
         <v>113860.5</v>
       </c>
-      <c r="BF2" t="n">
-        <v>116188.19486532</v>
-      </c>
-      <c r="BG2" t="n">
+      <c r="BE2">
+        <v>116188.19486531999</v>
+      </c>
+      <c r="BF2">
         <v>123112.162117204</v>
       </c>
-      <c r="BH2" t="n">
+      <c r="BG2">
         <v>129517.490179574</v>
       </c>
-      <c r="BI2" t="n">
+      <c r="BH2">
         <v>136945.195556758</v>
       </c>
-      <c r="BJ2" t="n">
-        <v>143222.317765953</v>
-      </c>
-      <c r="BK2" t="n">
+      <c r="BI2">
+        <v>143222.31776595299</v>
+      </c>
+      <c r="BJ2">
         <v>142758.10052409</v>
       </c>
-      <c r="BL2" t="n">
-        <v>143397.902792809</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>120474.186873697</v>
-      </c>
-      <c r="BN2" t="n">
-        <v>97117.9028880071</v>
-      </c>
-      <c r="BO2" t="n">
-        <v>86068.1767910587</v>
-      </c>
-      <c r="BP2" t="n">
-        <v>86818.8408857089</v>
-      </c>
-      <c r="BQ2" t="n">
+      <c r="BK2">
+        <v>143397.90279280901</v>
+      </c>
+      <c r="BL2">
+        <v>120474.18687369701</v>
+      </c>
+      <c r="BM2">
+        <v>97117.902888007098</v>
+      </c>
+      <c r="BN2">
+        <v>86068.176791058693</v>
+      </c>
+      <c r="BO2">
+        <v>86818.840885708894</v>
+      </c>
+      <c r="BP2">
         <v>84832.5</v>
       </c>
-      <c r="BR2" t="n">
+      <c r="BQ2">
         <v>88062.5</v>
       </c>
-      <c r="BS2" t="n">
+      <c r="BR2">
         <v>94567.5</v>
       </c>
-      <c r="BT2" t="n">
+      <c r="BS2">
         <v>107677.5</v>
       </c>
-      <c r="BU2" t="n">
+      <c r="BT2">
         <v>117517.5</v>
       </c>
-      <c r="BV2" t="n">
+      <c r="BU2">
         <v>128237.5</v>
       </c>
-      <c r="BW2" t="n">
+      <c r="BV2">
         <v>135077.5</v>
       </c>
-      <c r="BX2" t="n">
+      <c r="BW2">
         <v>138842.5</v>
       </c>
-      <c r="BY2" t="n">
+      <c r="BX2">
         <v>128732.5</v>
       </c>
-      <c r="BZ2" t="n">
+      <c r="BY2">
         <v>134142.5</v>
       </c>
-      <c r="CA2" t="n">
+      <c r="BZ2">
         <v>138060</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:BZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35:R35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -4361,249 +4370,269 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>14071.2</v>
       </c>
-      <c r="C2" t="n">
-        <v>75482.96128</v>
-      </c>
-      <c r="D2" t="n">
-        <v>149816.43584</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="C2">
+        <v>75482.961280000003</v>
+      </c>
+      <c r="D2">
+        <v>149816.43583999999</v>
+      </c>
+      <c r="E2">
         <v>126970.38728</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>126683.0156</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>125504</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>154028.16</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>185937.84</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>192154</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2">
         <v>157630</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>129063</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>125749</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>101761</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>90665</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2">
         <v>95170</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2">
         <v>85016</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2">
         <v>95092</v>
       </c>
-      <c r="S2" t="n">
+      <c r="S2">
         <v>88359</v>
       </c>
-      <c r="T2" t="n">
+      <c r="T2">
         <v>108506</v>
       </c>
-      <c r="U2" t="n">
+      <c r="U2">
         <v>121856</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V2">
         <v>137154</v>
       </c>
-      <c r="W2" t="n">
+      <c r="W2">
         <v>153550</v>
       </c>
-      <c r="X2" t="n">
+      <c r="X2">
         <v>142935</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="Y2">
         <v>131756</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="Z2">
         <v>133138</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AA2">
         <v>118351</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AB2">
         <v>94401</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AC2">
         <v>81396</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AD2">
         <v>102286</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AE2">
         <v>124110</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2">
         <v>124752</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG2">
         <v>132056</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AH2">
         <v>105946</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AI2">
         <v>82376</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AJ2">
         <v>88682</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AK2">
         <v>67094.5</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="AL2">
         <v>41246.5</v>
       </c>
-      <c r="AM2" t="n">
+      <c r="AM2">
         <v>42444</v>
       </c>
-      <c r="AN2" t="n">
+      <c r="AN2">
         <v>41653</v>
       </c>
-      <c r="AO2" t="n">
+      <c r="AO2">
         <v>35002.5</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="AP2">
         <v>30054</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AQ2">
         <v>27194</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AR2">
         <v>27081.5</v>
       </c>
-      <c r="AS2" t="n">
+      <c r="AS2">
         <v>25024.5</v>
       </c>
-      <c r="AT2" t="n">
+      <c r="AT2">
         <v>27856.5</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="AU2">
         <v>22961</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="AV2">
         <v>36491.75</v>
       </c>
-      <c r="AW2" t="n">
+      <c r="AW2">
         <v>42031.75</v>
       </c>
-      <c r="AX2" t="n">
+      <c r="AX2">
         <v>43460.25</v>
       </c>
-      <c r="AY2" t="n">
+      <c r="AY2">
         <v>48432.25</v>
       </c>
-      <c r="AZ2" t="n">
+      <c r="AZ2">
         <v>37697.5</v>
       </c>
-      <c r="BA2" t="n">
+      <c r="BA2">
         <v>29559.25</v>
       </c>
-      <c r="BB2" t="n">
+      <c r="BB2">
         <v>26960.5</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="BC2">
         <v>23403</v>
       </c>
-      <c r="BD2" t="n">
+      <c r="BD2">
         <v>21278.25</v>
       </c>
-      <c r="BE2" t="n">
+      <c r="BE2">
         <v>21534</v>
       </c>
-      <c r="BF2" t="n">
+      <c r="BF2">
         <v>21256.75</v>
       </c>
-      <c r="BG2" t="n">
+      <c r="BG2">
         <v>23190</v>
       </c>
-      <c r="BH2" t="n">
+      <c r="BH2">
         <v>26168.75</v>
       </c>
-      <c r="BI2" t="n">
+      <c r="BI2">
         <v>31687.75</v>
       </c>
-      <c r="BJ2" t="n">
+      <c r="BJ2">
         <v>35350.75</v>
       </c>
-      <c r="BK2" t="n">
+      <c r="BK2">
         <v>42145</v>
       </c>
-      <c r="BL2" t="n">
+      <c r="BL2">
         <v>44260.75</v>
       </c>
-      <c r="BM2" t="n">
+      <c r="BM2">
         <v>47122.25</v>
       </c>
-      <c r="BN2" t="n">
+      <c r="BN2">
         <v>51903.25</v>
       </c>
-      <c r="BO2" t="n">
+      <c r="BO2">
         <v>53066.5</v>
       </c>
-      <c r="BP2" t="n">
+      <c r="BP2">
         <v>42886.5</v>
       </c>
-      <c r="BQ2" t="n">
+      <c r="BQ2">
         <v>37454</v>
       </c>
-      <c r="BR2" t="n">
+      <c r="BR2">
         <v>52675.25</v>
       </c>
-      <c r="BS2" t="n">
+      <c r="BS2">
         <v>36326.75</v>
       </c>
-      <c r="BT2" t="n">
+      <c r="BT2">
         <v>36035.5</v>
       </c>
-      <c r="BU2" t="n">
+      <c r="BU2">
         <v>41753.5</v>
       </c>
-      <c r="BV2" t="n">
+      <c r="BV2">
         <v>50235.5</v>
       </c>
-      <c r="BW2" t="n">
+      <c r="BW2">
         <v>53252.5</v>
       </c>
-      <c r="BX2" t="n">
+      <c r="BX2">
         <v>47400</v>
       </c>
-      <c r="BY2" t="n">
+      <c r="BY2">
         <v>51653</v>
       </c>
-      <c r="BZ2" t="n">
+      <c r="BZ2">
         <v>57195</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a436561-34c6-48a8-833e-99c650fd3fe3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="25475540-9773-43a3-8df6-094be5ca1716" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005F8246D3F7C2B47A494A339FDF5CC4A" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ce096518759c6da43d5eeaaf714cf61">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a436561-34c6-48a8-833e-99c650fd3fe3" xmlns:ns3="25475540-9773-43a3-8df6-094be5ca1716" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="836b862547399ebb80cc78f9563635b2" ns2:_="" ns3:_="">
     <xsd:import namespace="7a436561-34c6-48a8-833e-99c650fd3fe3"/>
@@ -4858,34 +4887,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a436561-34c6-48a8-833e-99c650fd3fe3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="25475540-9773-43a3-8df6-094be5ca1716" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBAB0AF5-C639-46EB-94FB-83E8D1757393}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B9E4734-2BD5-49F7-8275-E886F32DA453}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7a436561-34c6-48a8-833e-99c650fd3fe3"/>
+    <ds:schemaRef ds:uri="25475540-9773-43a3-8df6-094be5ca1716"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7ABD5AA-7641-4724-9730-FBF5707A7D1E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7ABD5AA-7641-4724-9730-FBF5707A7D1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B9E4734-2BD5-49F7-8275-E886F32DA453}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBAB0AF5-C639-46EB-94FB-83E8D1757393}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7a436561-34c6-48a8-833e-99c650fd3fe3"/>
+    <ds:schemaRef ds:uri="25475540-9773-43a3-8df6-094be5ca1716"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>